<commit_message>
added alternative method for post returns
</commit_message>
<xml_diff>
--- a/ProblemTest.xlsx
+++ b/ProblemTest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="1" state="visible" r:id="rId2"/>
@@ -164,10 +164,10 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.86"/>
   </cols>
@@ -209,7 +209,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0.005</v>
+        <v>0.05</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0.08</v>
@@ -255,11 +255,11 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -361,11 +361,11 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.86"/>

</xml_diff>